<commit_message>
Google Trends India 2023
</commit_message>
<xml_diff>
--- a/Google Trends/interest_over_time.xlsx
+++ b/Google Trends/interest_over_time.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivektiwari/Code/Programming/visualizetrends/Google Trends/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8777820-6820-E541-8DE1-013E3FEFEE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F68190D-28F2-C440-8C29-E1BF90C121B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>date</t>
   </si>
@@ -68,6 +68,27 @@
   </si>
   <si>
     <t>G20 Summit</t>
+  </si>
+  <si>
+    <t>Manipur</t>
+  </si>
+  <si>
+    <t>Giorgia Meloni</t>
+  </si>
+  <si>
+    <t>Election Result</t>
+  </si>
+  <si>
+    <t>Bharat Jodo Yatra</t>
+  </si>
+  <si>
+    <t>UCC</t>
+  </si>
+  <si>
+    <t>Justin Trudeau</t>
+  </si>
+  <si>
+    <t>I.N.D.I.A</t>
   </si>
 </sst>
 </file>
@@ -924,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:W51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,9 +969,12 @@
     <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -999,8 +1023,29 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44927</v>
       </c>
@@ -1049,8 +1094,29 @@
       <c r="P2" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q2">
+        <v>7</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>100</v>
+      </c>
+      <c r="U2">
+        <v>2</v>
+      </c>
+      <c r="V2">
+        <v>2</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44934</v>
       </c>
@@ -1099,8 +1165,29 @@
       <c r="P3" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3">
+        <v>8</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>99</v>
+      </c>
+      <c r="U3">
+        <v>3</v>
+      </c>
+      <c r="V3">
+        <v>2</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>44941</v>
       </c>
@@ -1149,8 +1236,29 @@
       <c r="P4" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q4">
+        <v>7</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>77</v>
+      </c>
+      <c r="U4">
+        <v>2</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>44948</v>
       </c>
@@ -1199,8 +1307,29 @@
       <c r="P5" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5">
+        <v>7</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>86</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+      <c r="V5">
+        <v>2</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>44955</v>
       </c>
@@ -1249,8 +1378,29 @@
       <c r="P6" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q6">
+        <v>7</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>3</v>
+      </c>
+      <c r="T6">
+        <v>66</v>
+      </c>
+      <c r="U6">
+        <v>2</v>
+      </c>
+      <c r="V6">
+        <v>2</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>44962</v>
       </c>
@@ -1299,8 +1449,29 @@
       <c r="P7" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q7">
+        <v>7</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>18</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="V7">
+        <v>2</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>44969</v>
       </c>
@@ -1349,8 +1520,29 @@
       <c r="P8" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q8">
+        <v>8</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>2</v>
+      </c>
+      <c r="T8">
+        <v>9</v>
+      </c>
+      <c r="U8">
+        <v>2</v>
+      </c>
+      <c r="V8">
+        <v>2</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>44976</v>
       </c>
@@ -1399,8 +1591,29 @@
       <c r="P9" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q9">
+        <v>8</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>2</v>
+      </c>
+      <c r="T9">
+        <v>8</v>
+      </c>
+      <c r="U9">
+        <v>3</v>
+      </c>
+      <c r="V9">
+        <v>2</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44983</v>
       </c>
@@ -1449,8 +1662,29 @@
       <c r="P10" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q10">
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <v>23</v>
+      </c>
+      <c r="S10">
+        <v>22</v>
+      </c>
+      <c r="T10">
+        <v>10</v>
+      </c>
+      <c r="U10">
+        <v>2</v>
+      </c>
+      <c r="V10">
+        <v>2</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44990</v>
       </c>
@@ -1499,8 +1733,29 @@
       <c r="P11" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q11">
+        <v>6</v>
+      </c>
+      <c r="R11">
+        <v>5</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>4</v>
+      </c>
+      <c r="U11">
+        <v>3</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>44997</v>
       </c>
@@ -1549,8 +1804,29 @@
       <c r="P12" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q12">
+        <v>7</v>
+      </c>
+      <c r="R12">
+        <v>2</v>
+      </c>
+      <c r="S12">
+        <v>4</v>
+      </c>
+      <c r="T12">
+        <v>5</v>
+      </c>
+      <c r="U12">
+        <v>2</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>45004</v>
       </c>
@@ -1599,8 +1875,29 @@
       <c r="P13" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q13">
+        <v>7</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>9</v>
+      </c>
+      <c r="U13">
+        <v>3</v>
+      </c>
+      <c r="V13">
+        <v>2</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>45011</v>
       </c>
@@ -1649,8 +1946,29 @@
       <c r="P14" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q14">
+        <v>8</v>
+      </c>
+      <c r="R14">
+        <v>2</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>5</v>
+      </c>
+      <c r="U14">
+        <v>2</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>45018</v>
       </c>
@@ -1699,8 +2017,29 @@
       <c r="P15" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q15">
+        <v>7</v>
+      </c>
+      <c r="R15">
+        <v>2</v>
+      </c>
+      <c r="S15">
+        <v>2</v>
+      </c>
+      <c r="T15">
+        <v>2</v>
+      </c>
+      <c r="U15">
+        <v>2</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>45025</v>
       </c>
@@ -1749,8 +2088,29 @@
       <c r="P16" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q16">
+        <v>8</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>2</v>
+      </c>
+      <c r="U16">
+        <v>2</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>45032</v>
       </c>
@@ -1799,8 +2159,29 @@
       <c r="P17" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q17">
+        <v>7</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>3</v>
+      </c>
+      <c r="U17">
+        <v>2</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>45039</v>
       </c>
@@ -1849,8 +2230,29 @@
       <c r="P18" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q18">
+        <v>7</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>2</v>
+      </c>
+      <c r="T18">
+        <v>3</v>
+      </c>
+      <c r="U18">
+        <v>2</v>
+      </c>
+      <c r="V18">
+        <v>2</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>45046</v>
       </c>
@@ -1899,8 +2301,29 @@
       <c r="P19" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q19">
+        <v>16</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>2</v>
+      </c>
+      <c r="T19">
+        <v>3</v>
+      </c>
+      <c r="U19">
+        <v>3</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>45053</v>
       </c>
@@ -1949,8 +2372,29 @@
       <c r="P20" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q20">
+        <v>12</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>95</v>
+      </c>
+      <c r="T20">
+        <v>6</v>
+      </c>
+      <c r="U20">
+        <v>2</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>45060</v>
       </c>
@@ -1999,8 +2443,29 @@
       <c r="P21" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q21">
+        <v>7</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>14</v>
+      </c>
+      <c r="T21">
+        <v>7</v>
+      </c>
+      <c r="U21">
+        <v>3</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>45067</v>
       </c>
@@ -2049,8 +2514,29 @@
       <c r="P22" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q22">
+        <v>7</v>
+      </c>
+      <c r="R22">
+        <v>10</v>
+      </c>
+      <c r="S22">
+        <v>2</v>
+      </c>
+      <c r="T22">
+        <v>5</v>
+      </c>
+      <c r="U22">
+        <v>2</v>
+      </c>
+      <c r="V22">
+        <v>3</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>45074</v>
       </c>
@@ -2099,8 +2585,29 @@
       <c r="P23" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q23">
+        <v>11</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>2</v>
+      </c>
+      <c r="T23">
+        <v>3</v>
+      </c>
+      <c r="U23">
+        <v>2</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>45081</v>
       </c>
@@ -2149,8 +2656,29 @@
       <c r="P24" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q24">
+        <v>10</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>3</v>
+      </c>
+      <c r="U24">
+        <v>2</v>
+      </c>
+      <c r="V24">
+        <v>2</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>45088</v>
       </c>
@@ -2199,8 +2727,29 @@
       <c r="P25" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q25">
+        <v>11</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>2</v>
+      </c>
+      <c r="T25">
+        <v>4</v>
+      </c>
+      <c r="U25">
+        <v>14</v>
+      </c>
+      <c r="V25">
+        <v>2</v>
+      </c>
+      <c r="W25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>45095</v>
       </c>
@@ -2249,8 +2798,29 @@
       <c r="P26" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q26">
+        <v>12</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <v>4</v>
+      </c>
+      <c r="U26">
+        <v>16</v>
+      </c>
+      <c r="V26">
+        <v>2</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>45102</v>
       </c>
@@ -2299,8 +2869,29 @@
       <c r="P27" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q27">
+        <v>14</v>
+      </c>
+      <c r="R27">
+        <v>4</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27">
+        <v>3</v>
+      </c>
+      <c r="U27">
+        <v>100</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>45109</v>
       </c>
@@ -2349,8 +2940,29 @@
       <c r="P28" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q28">
+        <v>11</v>
+      </c>
+      <c r="R28">
+        <v>2</v>
+      </c>
+      <c r="S28">
+        <v>1</v>
+      </c>
+      <c r="T28">
+        <v>3</v>
+      </c>
+      <c r="U28">
+        <v>98</v>
+      </c>
+      <c r="V28">
+        <v>2</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>45116</v>
       </c>
@@ -2399,8 +3011,29 @@
       <c r="P29" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q29">
+        <v>8</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>12</v>
+      </c>
+      <c r="T29">
+        <v>3</v>
+      </c>
+      <c r="U29">
+        <v>65</v>
+      </c>
+      <c r="V29">
+        <v>2</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>45123</v>
       </c>
@@ -2449,8 +3082,29 @@
       <c r="P30" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q30">
+        <v>100</v>
+      </c>
+      <c r="R30">
+        <v>2</v>
+      </c>
+      <c r="S30">
+        <v>2</v>
+      </c>
+      <c r="T30">
+        <v>4</v>
+      </c>
+      <c r="U30">
+        <v>31</v>
+      </c>
+      <c r="V30">
+        <v>2</v>
+      </c>
+      <c r="W30">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>45130</v>
       </c>
@@ -2499,8 +3153,29 @@
       <c r="P31" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q31">
+        <v>45</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+      <c r="T31">
+        <v>6</v>
+      </c>
+      <c r="U31">
+        <v>18</v>
+      </c>
+      <c r="V31">
+        <v>2</v>
+      </c>
+      <c r="W31">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>45137</v>
       </c>
@@ -2549,8 +3224,29 @@
       <c r="P32" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q32">
+        <v>17</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <v>6</v>
+      </c>
+      <c r="U32">
+        <v>11</v>
+      </c>
+      <c r="V32">
+        <v>23</v>
+      </c>
+      <c r="W32">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>45144</v>
       </c>
@@ -2599,8 +3295,29 @@
       <c r="P33" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q33">
+        <v>16</v>
+      </c>
+      <c r="R33">
+        <v>1</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="T33">
+        <v>9</v>
+      </c>
+      <c r="U33">
+        <v>9</v>
+      </c>
+      <c r="V33">
+        <v>5</v>
+      </c>
+      <c r="W33">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>45151</v>
       </c>
@@ -2649,8 +3366,29 @@
       <c r="P34" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q34">
+        <v>11</v>
+      </c>
+      <c r="R34">
+        <v>1</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+      <c r="T34">
+        <v>8</v>
+      </c>
+      <c r="U34">
+        <v>7</v>
+      </c>
+      <c r="V34">
+        <v>2</v>
+      </c>
+      <c r="W34">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>45158</v>
       </c>
@@ -2699,8 +3437,29 @@
       <c r="P35" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q35">
+        <v>9</v>
+      </c>
+      <c r="R35">
+        <v>1</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
+      </c>
+      <c r="T35">
+        <v>4</v>
+      </c>
+      <c r="U35">
+        <v>6</v>
+      </c>
+      <c r="V35">
+        <v>2</v>
+      </c>
+      <c r="W35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>45165</v>
       </c>
@@ -2749,8 +3508,29 @@
       <c r="P36" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q36">
+        <v>7</v>
+      </c>
+      <c r="R36">
+        <v>1</v>
+      </c>
+      <c r="S36">
+        <v>1</v>
+      </c>
+      <c r="T36">
+        <v>3</v>
+      </c>
+      <c r="U36">
+        <v>7</v>
+      </c>
+      <c r="V36">
+        <v>3</v>
+      </c>
+      <c r="W36">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>45172</v>
       </c>
@@ -2799,8 +3579,29 @@
       <c r="P37" s="3">
         <v>100</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q37">
+        <v>7</v>
+      </c>
+      <c r="R37">
+        <v>14</v>
+      </c>
+      <c r="S37">
+        <v>8</v>
+      </c>
+      <c r="T37">
+        <v>10</v>
+      </c>
+      <c r="U37">
+        <v>6</v>
+      </c>
+      <c r="V37">
+        <v>19</v>
+      </c>
+      <c r="W37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>45179</v>
       </c>
@@ -2849,8 +3650,29 @@
       <c r="P38" s="3">
         <v>58</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q38">
+        <v>6</v>
+      </c>
+      <c r="R38">
+        <v>100</v>
+      </c>
+      <c r="S38">
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <v>4</v>
+      </c>
+      <c r="U38">
+        <v>5</v>
+      </c>
+      <c r="V38">
+        <v>99</v>
+      </c>
+      <c r="W38">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>45186</v>
       </c>
@@ -2899,8 +3721,29 @@
       <c r="P39" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q39">
+        <v>7</v>
+      </c>
+      <c r="R39">
+        <v>49</v>
+      </c>
+      <c r="S39">
+        <v>3</v>
+      </c>
+      <c r="T39">
+        <v>3</v>
+      </c>
+      <c r="U39">
+        <v>5</v>
+      </c>
+      <c r="V39">
+        <v>100</v>
+      </c>
+      <c r="W39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>45193</v>
       </c>
@@ -2949,8 +3792,29 @@
       <c r="P40" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q40">
+        <v>9</v>
+      </c>
+      <c r="R40">
+        <v>17</v>
+      </c>
+      <c r="S40">
+        <v>2</v>
+      </c>
+      <c r="T40">
+        <v>4</v>
+      </c>
+      <c r="U40">
+        <v>5</v>
+      </c>
+      <c r="V40">
+        <v>42</v>
+      </c>
+      <c r="W40">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>45200</v>
       </c>
@@ -2999,8 +3863,29 @@
       <c r="P41" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q41">
+        <v>8</v>
+      </c>
+      <c r="R41">
+        <v>11</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <v>3</v>
+      </c>
+      <c r="U41">
+        <v>4</v>
+      </c>
+      <c r="V41">
+        <v>35</v>
+      </c>
+      <c r="W41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>45207</v>
       </c>
@@ -3049,8 +3934,29 @@
       <c r="P42" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q42">
+        <v>7</v>
+      </c>
+      <c r="R42">
+        <v>8</v>
+      </c>
+      <c r="S42">
+        <v>1</v>
+      </c>
+      <c r="T42">
+        <v>3</v>
+      </c>
+      <c r="U42">
+        <v>5</v>
+      </c>
+      <c r="V42">
+        <v>11</v>
+      </c>
+      <c r="W42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>45214</v>
       </c>
@@ -3099,8 +4005,29 @@
       <c r="P43" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q43">
+        <v>7</v>
+      </c>
+      <c r="R43">
+        <v>37</v>
+      </c>
+      <c r="S43">
+        <v>1</v>
+      </c>
+      <c r="T43">
+        <v>4</v>
+      </c>
+      <c r="U43">
+        <v>4</v>
+      </c>
+      <c r="V43">
+        <v>21</v>
+      </c>
+      <c r="W43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>45221</v>
       </c>
@@ -3149,8 +4076,29 @@
       <c r="P44" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q44">
+        <v>7</v>
+      </c>
+      <c r="R44">
+        <v>15</v>
+      </c>
+      <c r="S44">
+        <v>1</v>
+      </c>
+      <c r="T44">
+        <v>2</v>
+      </c>
+      <c r="U44">
+        <v>3</v>
+      </c>
+      <c r="V44">
+        <v>16</v>
+      </c>
+      <c r="W44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>45228</v>
       </c>
@@ -3199,8 +4147,29 @@
       <c r="P45" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q45">
+        <v>7</v>
+      </c>
+      <c r="R45">
+        <v>4</v>
+      </c>
+      <c r="S45">
+        <v>1</v>
+      </c>
+      <c r="T45">
+        <v>1</v>
+      </c>
+      <c r="U45">
+        <v>3</v>
+      </c>
+      <c r="V45">
+        <v>5</v>
+      </c>
+      <c r="W45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45235</v>
       </c>
@@ -3249,8 +4218,29 @@
       <c r="P46" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q46">
+        <v>6</v>
+      </c>
+      <c r="R46">
+        <v>2</v>
+      </c>
+      <c r="S46">
+        <v>2</v>
+      </c>
+      <c r="T46">
+        <v>2</v>
+      </c>
+      <c r="U46">
+        <v>4</v>
+      </c>
+      <c r="V46">
+        <v>2</v>
+      </c>
+      <c r="W46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>45242</v>
       </c>
@@ -3299,8 +4289,29 @@
       <c r="P47" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q47">
+        <v>4</v>
+      </c>
+      <c r="R47">
+        <v>2</v>
+      </c>
+      <c r="S47">
+        <v>3</v>
+      </c>
+      <c r="T47">
+        <v>2</v>
+      </c>
+      <c r="U47">
+        <v>4</v>
+      </c>
+      <c r="V47">
+        <v>10</v>
+      </c>
+      <c r="W47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>45249</v>
       </c>
@@ -3349,8 +4360,29 @@
       <c r="P48" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q48">
+        <v>7</v>
+      </c>
+      <c r="R48">
+        <v>2</v>
+      </c>
+      <c r="S48">
+        <v>4</v>
+      </c>
+      <c r="T48">
+        <v>2</v>
+      </c>
+      <c r="U48">
+        <v>4</v>
+      </c>
+      <c r="V48">
+        <v>2</v>
+      </c>
+      <c r="W48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>45256</v>
       </c>
@@ -3399,8 +4431,29 @@
       <c r="P49" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q49">
+        <v>7</v>
+      </c>
+      <c r="R49">
+        <v>33</v>
+      </c>
+      <c r="S49">
+        <v>8</v>
+      </c>
+      <c r="T49">
+        <v>3</v>
+      </c>
+      <c r="U49">
+        <v>4</v>
+      </c>
+      <c r="V49">
+        <v>4</v>
+      </c>
+      <c r="W49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>45263</v>
       </c>
@@ -3449,8 +4502,29 @@
       <c r="P50" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q50">
+        <v>9</v>
+      </c>
+      <c r="R50">
+        <v>30</v>
+      </c>
+      <c r="S50">
+        <v>100</v>
+      </c>
+      <c r="T50">
+        <v>3</v>
+      </c>
+      <c r="U50">
+        <v>4</v>
+      </c>
+      <c r="V50">
+        <v>1</v>
+      </c>
+      <c r="W50">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>45270</v>
       </c>
@@ -3497,6 +4571,27 @@
         <v>8</v>
       </c>
       <c r="P51" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q51">
+        <v>7</v>
+      </c>
+      <c r="R51">
+        <v>7</v>
+      </c>
+      <c r="S51">
+        <v>3</v>
+      </c>
+      <c r="T51">
+        <v>3</v>
+      </c>
+      <c r="U51">
+        <v>4</v>
+      </c>
+      <c r="V51">
+        <v>1</v>
+      </c>
+      <c r="W51">
         <v>3</v>
       </c>
     </row>

</xml_diff>